<commit_message>
[Sprint 1][Generic] - small corrections on Glossary
</commit_message>
<xml_diff>
--- a/docs/Glossary/Glossary.xlsx
+++ b/docs/Glossary/Glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myisepipp.sharepoint.com/teams/2NB-LAPR4-ISEP365Group/Shared Documents/General/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myisepipp-my.sharepoint.com/personal/1100358_isep_ipp_pt/Documents/LEI/2_Ano_2_Sem/LAPR4/sem4pi-22-23-49/docs/Glossary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="571" documentId="8_{DE2A04C6-A3AB-3646-91C7-13FC4BF5E613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8BC6D14-AE7D-F849-B055-24C06009880C}"/>
+  <xr:revisionPtr revIDLastSave="575" documentId="8_{DE2A04C6-A3AB-3646-91C7-13FC4BF5E613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BADD7601-0B4B-9646-8442-DCF0C77F826F}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-460" windowWidth="38400" windowHeight="21100" xr2:uid="{42D5D6CD-F1CD-DB4E-B209-846E2890D1BF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{42D5D6CD-F1CD-DB4E-B209-846E2890D1BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="1" r:id="rId1"/>
@@ -413,9 +413,6 @@
     <t>The user that created a meeting cancelled it.</t>
   </si>
   <si>
-    <t>Schedulle Meeting</t>
-  </si>
-  <si>
     <t>Agendar Reunião</t>
   </si>
   <si>
@@ -456,9 +453,6 @@
   </si>
   <si>
     <t>Inscrição rejeitada</t>
-  </si>
-  <si>
-    <t>Update Schedulle</t>
   </si>
   <si>
     <t>Atualizar Marcação</t>
@@ -643,15 +637,9 @@
     <t>Exam Layout</t>
   </si>
   <si>
-    <t>Exame Question</t>
-  </si>
-  <si>
     <t>Exam Solution</t>
   </si>
   <si>
-    <t>Exame Feedback</t>
-  </si>
-  <si>
     <t>Exam Grading</t>
   </si>
   <si>
@@ -950,6 +938,18 @@
   </si>
   <si>
     <t>The individual or entity that has primary ownership and control over a particular digital board</t>
+  </si>
+  <si>
+    <t>Exam Feedback</t>
+  </si>
+  <si>
+    <t>Exam Question</t>
+  </si>
+  <si>
+    <t>Schedule Meeting</t>
+  </si>
+  <si>
+    <t>Update Schedule</t>
   </si>
 </sst>
 </file>
@@ -1346,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259ED946-36CD-BE4D-8726-A8102DC76C67}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1397,68 +1397,68 @@
     </row>
     <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" t="s">
         <v>133</v>
       </c>
-      <c r="B4" t="s">
-        <v>134</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>181</v>
-      </c>
-      <c r="B5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="B6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1474,13 +1474,13 @@
     </row>
     <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1496,24 +1496,24 @@
     </row>
     <row r="13" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B13" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B14" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1529,13 +1529,13 @@
     </row>
     <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" t="s">
         <v>127</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1551,24 +1551,24 @@
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="B19" t="s">
-        <v>170</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1584,13 +1584,13 @@
     </row>
     <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B21" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1617,57 +1617,57 @@
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B24" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B25" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B26" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B27" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B28" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1683,13 +1683,13 @@
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B30" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1716,13 +1716,13 @@
     </row>
     <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B33" t="s">
+        <v>171</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>172</v>
-      </c>
-      <c r="B33" t="s">
-        <v>173</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1738,13 +1738,13 @@
     </row>
     <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B35" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1760,76 +1760,76 @@
     </row>
     <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B37" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B38" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B39" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B40" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B41" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B43" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1845,35 +1845,35 @@
     </row>
     <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B45" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>199</v>
+        <v>296</v>
       </c>
       <c r="B46" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>197</v>
+        <v>297</v>
       </c>
       <c r="B47" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1911,13 +1911,13 @@
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>184</v>
+      </c>
+      <c r="B51" t="s">
+        <v>185</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="B51" t="s">
-        <v>187</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1933,79 +1933,79 @@
     </row>
     <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B53" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B54" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B55" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B56" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B57" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B58" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B59" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2032,13 +2032,13 @@
     </row>
     <row r="62" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B62" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2065,35 +2065,35 @@
     </row>
     <row r="65" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>152</v>
+      </c>
+      <c r="B65" t="s">
+        <v>153</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="B65" t="s">
-        <v>155</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" t="s">
+        <v>174</v>
+      </c>
+      <c r="C66" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="B66" t="s">
-        <v>176</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>158</v>
+      </c>
+      <c r="B67" t="s">
+        <v>159</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="B67" t="s">
-        <v>161</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2109,13 +2109,13 @@
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>147</v>
+      </c>
+      <c r="B69" t="s">
+        <v>148</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="B69" t="s">
-        <v>150</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2142,13 +2142,13 @@
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B72" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2164,35 +2164,35 @@
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>129</v>
+      </c>
+      <c r="B74" t="s">
         <v>130</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B75" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>135</v>
+      </c>
+      <c r="B76" t="s">
         <v>136</v>
       </c>
-      <c r="B76" t="s">
-        <v>137</v>
-      </c>
       <c r="C76" s="4" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2230,54 +2230,54 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>124</v>
+      </c>
+      <c r="B80" t="s">
         <v>125</v>
-      </c>
-      <c r="B80" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B81" t="s">
         <v>77</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B82" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B83" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B84" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2304,35 +2304,35 @@
     </row>
     <row r="87" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>298</v>
+      </c>
+      <c r="B87" t="s">
         <v>123</v>
       </c>
-      <c r="B87" t="s">
-        <v>124</v>
-      </c>
       <c r="C87" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>161</v>
+      </c>
+      <c r="B88" t="s">
+        <v>162</v>
+      </c>
+      <c r="C88" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="B88" t="s">
-        <v>164</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B89" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2348,13 +2348,13 @@
     </row>
     <row r="91" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>155</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C91" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2425,35 +2425,35 @@
     </row>
     <row r="98" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B98" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>164</v>
+      </c>
+      <c r="B99" t="s">
+        <v>165</v>
+      </c>
+      <c r="C99" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="B99" t="s">
-        <v>167</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>299</v>
+      </c>
+      <c r="B100" t="s">
+        <v>137</v>
+      </c>
+      <c r="C100" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="B100" t="s">
-        <v>139</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2487,17 +2487,17 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2506,18 +2506,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2665,25 +2665,25 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F43674B0-2D06-4B1D-A297-9905C5508570}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{468F12D2-F208-4C37-974B-462588DBE2CB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="0140ed85-122a-4fcb-b20c-e3a017deab9b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{468F12D2-F208-4C37-974B-462588DBE2CB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F43674B0-2D06-4B1D-A297-9905C5508570}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="0140ed85-122a-4fcb-b20c-e3a017deab9b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>